<commit_message>
- Nullpunkt Kreis Hamm aktualisiert (der Punkt Unna scheint für die Mehrzahl oder alle Bürgermeistereien in Hamm zu gelten)
- kleinere Formatierungsänderungen _vorlage_net
- Vermessungsnetz Camen ergänzt
- kleinere Korrekturen an Vermessungsnetzen
</commit_message>
<xml_diff>
--- a/_vorlage_net.xlsx
+++ b/_vorlage_net.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57FD40D-D0FA-4011-9960-94B988C31573}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF78E39D-F290-4B8A-A317-3F9D42F6FB04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17" yWindow="420" windowWidth="32674" windowHeight="17494" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="420" windowWidth="32674" windowHeight="17494" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rechnung goniom. Koord." sheetId="1" r:id="rId1"/>
+    <sheet name="Einstellungen" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Berechnung goniometrische Coordinate</t>
   </si>
@@ -95,6 +96,15 @@
   </si>
   <si>
     <t>25 II Wandhofen</t>
+  </si>
+  <si>
+    <t>Flur</t>
+  </si>
+  <si>
+    <t>Ignoriere Koordinaten</t>
+  </si>
+  <si>
+    <t>Spiegeln</t>
   </si>
 </sst>
 </file>
@@ -171,7 +181,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -249,11 +259,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -307,6 +326,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -634,7 +654,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="49" zoomScaleNormal="49" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="AC17" sqref="AC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.42578125" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -661,10 +681,13 @@
     <col min="22" max="22" width="7.85546875" style="5" customWidth="1"/>
     <col min="23" max="23" width="4.85546875" style="6" customWidth="1"/>
     <col min="24" max="24" width="3.140625" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" style="5"/>
     <col min="26" max="26" width="3.85546875" style="6" customWidth="1"/>
     <col min="27" max="27" width="2.640625" customWidth="1"/>
+    <col min="28" max="28" width="10.42578125" style="5"/>
     <col min="29" max="29" width="5" customWidth="1"/>
     <col min="30" max="30" width="2.5" customWidth="1"/>
+    <col min="31" max="31" width="10.42578125" style="5"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.45">
@@ -679,49 +702,49 @@
       <c r="B2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26" t="s">
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="27" t="s">
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
+      <c r="K2" s="27"/>
+      <c r="L2" s="27"/>
+      <c r="M2" s="27"/>
       <c r="N2" s="9"/>
-      <c r="O2" s="26" t="s">
+      <c r="O2" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26" t="s">
+      <c r="P2" s="27"/>
+      <c r="Q2" s="27"/>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26" t="s">
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="27"/>
+      <c r="AE2" s="27"/>
     </row>
     <row r="3" spans="1:31" s="10" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="7"/>
@@ -744,37 +767,37 @@
       <c r="H3" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="26"/>
-      <c r="K3" s="26"/>
-      <c r="L3" s="26"/>
-      <c r="M3" s="26"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="27"/>
       <c r="N3" s="12"/>
-      <c r="O3" s="26"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="26"/>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26" t="s">
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="27"/>
+      <c r="S3" s="27"/>
+      <c r="T3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="U3" s="26"/>
-      <c r="V3" s="26"/>
-      <c r="W3" s="26" t="s">
+      <c r="U3" s="27"/>
+      <c r="V3" s="27"/>
+      <c r="W3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="X3" s="26"/>
-      <c r="Y3" s="26"/>
-      <c r="Z3" s="26" t="s">
+      <c r="X3" s="27"/>
+      <c r="Y3" s="27"/>
+      <c r="Z3" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="AA3" s="26"/>
-      <c r="AB3" s="26"/>
-      <c r="AC3" s="26" t="s">
+      <c r="AA3" s="27"/>
+      <c r="AB3" s="27"/>
+      <c r="AC3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="AD3" s="26"/>
-      <c r="AE3" s="26"/>
+      <c r="AD3" s="27"/>
+      <c r="AE3" s="27"/>
     </row>
     <row r="4" spans="1:31" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="13"/>
@@ -782,9 +805,9 @@
         <v>19</v>
       </c>
       <c r="C4" s="15"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
       <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="18"/>
@@ -801,13 +824,13 @@
       <c r="V4" s="20"/>
       <c r="W4" s="18"/>
       <c r="X4" s="18"/>
-      <c r="Y4" s="18"/>
+      <c r="Y4" s="20"/>
       <c r="Z4" s="18"/>
       <c r="AA4" s="18"/>
-      <c r="AB4" s="18"/>
+      <c r="AB4" s="20"/>
       <c r="AC4" s="18"/>
       <c r="AD4" s="18"/>
-      <c r="AE4" s="18"/>
+      <c r="AE4" s="20"/>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
@@ -816,13 +839,13 @@
       <c r="AA5" t="s">
         <v>15</v>
       </c>
-      <c r="AB5">
+      <c r="AB5" s="5">
         <v>0</v>
       </c>
       <c r="AD5" t="s">
         <v>16</v>
       </c>
-      <c r="AE5">
+      <c r="AE5" s="5">
         <v>0</v>
       </c>
     </row>
@@ -833,13 +856,13 @@
       <c r="AA6" t="s">
         <v>15</v>
       </c>
-      <c r="AB6">
+      <c r="AB6" s="5">
         <v>251.83</v>
       </c>
       <c r="AD6" t="s">
         <v>16</v>
       </c>
-      <c r="AE6">
+      <c r="AE6" s="5">
         <v>1027.71</v>
       </c>
     </row>
@@ -847,8 +870,6 @@
       <c r="B8" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="AB8" s="5"/>
-      <c r="AE8" s="5"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
@@ -891,13 +912,13 @@
       <c r="AA11" t="s">
         <v>15</v>
       </c>
-      <c r="AB11">
+      <c r="AB11" s="5">
         <v>1589.65</v>
       </c>
       <c r="AD11" t="s">
         <v>16</v>
       </c>
-      <c r="AE11">
+      <c r="AE11" s="5">
         <v>2499.89</v>
       </c>
     </row>
@@ -913,13 +934,13 @@
       <c r="AA12" t="s">
         <v>15</v>
       </c>
-      <c r="AB12">
+      <c r="AB12" s="5">
         <v>1847.81</v>
       </c>
       <c r="AD12" t="s">
         <v>16</v>
       </c>
-      <c r="AE12">
+      <c r="AE12" s="5">
         <v>2445.91</v>
       </c>
     </row>
@@ -939,6 +960,41 @@
     <mergeCell ref="AC3:AE3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F924D68-3404-446E-9602-DC3C29EDF9EF}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A1" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>